<commit_message>
Atualização após o clássico.
Expectativa é que eu consigo montar uma tabela com algumas estatísticas como posse de bola, chutes, escanteio etc.
</commit_message>
<xml_diff>
--- a/data/matches_FLA2023.xlsx
+++ b/data/matches_FLA2023.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="185">
   <si>
     <t xml:space="preserve">id_match</t>
   </si>
@@ -480,6 +480,15 @@
   </si>
   <si>
     <t xml:space="preserve">2023-06-01 20:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campeonato Brasileiro - Round 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-06-05 20:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">gols</t>
@@ -578,7 +587,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -599,11 +608,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -661,7 +665,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,13 +686,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
+      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.18"/>
@@ -1658,6 +1662,32 @@
         <v>152</v>
       </c>
       <c r="H37" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1677,13 +1707,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -1695,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,10 +1736,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,10 +1747,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,10 +1758,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,10 +1769,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,10 +1780,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,10 +1791,10 @@
         <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,10 +1802,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,10 +1813,10 @@
         <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,10 +1824,10 @@
         <v>23</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,21 +1835,21 @@
         <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,10 +1857,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,10 +1868,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,10 +1879,10 @@
         <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,10 +1890,10 @@
         <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,10 +1901,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,10 +1912,10 @@
         <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,10 +1923,10 @@
         <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,10 +1934,10 @@
         <v>46</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1915,10 +1945,10 @@
         <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,10 +1956,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,10 +1967,10 @@
         <v>51</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,10 +1978,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1959,10 +1989,10 @@
         <v>51</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,10 +2000,10 @@
         <v>55</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,10 +2011,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,10 +2022,10 @@
         <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,10 +2033,10 @@
         <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,10 +2044,10 @@
         <v>75</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,10 +2055,10 @@
         <v>79</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,10 +2066,10 @@
         <v>79</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,10 +2077,10 @@
         <v>79</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,10 +2088,10 @@
         <v>82</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,10 +2099,10 @@
         <v>82</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,10 +2110,10 @@
         <v>82</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,10 +2121,10 @@
         <v>85</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2102,10 +2132,10 @@
         <v>85</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,10 +2143,10 @@
         <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,10 +2154,10 @@
         <v>93</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,10 +2165,10 @@
         <v>101</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,10 +2176,10 @@
         <v>101</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,10 +2187,10 @@
         <v>101</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,10 +2198,10 @@
         <v>105</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,10 +2209,10 @@
         <v>105</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,10 +2220,10 @@
         <v>109</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,10 +2231,10 @@
         <v>114</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,10 +2242,10 @@
         <v>114</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,10 +2253,10 @@
         <v>114</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,10 +2264,10 @@
         <v>114</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,10 +2275,10 @@
         <v>114</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,10 +2286,10 @@
         <v>114</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,10 +2297,10 @@
         <v>114</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,10 +2308,10 @@
         <v>114</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,10 +2319,10 @@
         <v>117</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,10 +2330,10 @@
         <v>117</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,10 +2341,10 @@
         <v>120</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,10 +2352,10 @@
         <v>125</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,10 +2363,10 @@
         <v>130</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,10 +2374,10 @@
         <v>130</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,10 +2385,10 @@
         <v>134</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,10 +2396,10 @@
         <v>134</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,10 +2407,10 @@
         <v>134</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,10 +2418,10 @@
         <v>142</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,10 +2429,10 @@
         <v>145</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,10 +2440,10 @@
         <v>148</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,10 +2451,10 @@
         <v>150</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,10 +2462,54 @@
         <v>150</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C68" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização após jogo da libertadores
</commit_message>
<xml_diff>
--- a/data/matches_FLA2023.xlsx
+++ b/data/matches_FLA2023.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="188">
   <si>
     <t xml:space="preserve">id_match</t>
   </si>
@@ -489,6 +489,15 @@
   </si>
   <si>
     <t xml:space="preserve">2023-06-05 20:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIB5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copa Libertadores da América - Round 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-06-08 21:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">gols</t>
@@ -686,13 +695,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="1" sqref="A73:C74 A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.18"/>
@@ -1688,6 +1697,32 @@
         <v>155</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1707,13 +1742,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73:C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -1725,10 +1760,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,10 +1771,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,10 +1782,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,10 +1793,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,10 +1804,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>163</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,10 +1815,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,10 +1826,10 @@
         <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,10 +1837,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,10 +1848,10 @@
         <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,10 +1859,10 @@
         <v>23</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,10 +1870,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,10 +1881,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,10 +1892,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,10 +1903,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,10 +1914,10 @@
         <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,10 +1925,10 @@
         <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,10 +1936,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,10 +1947,10 @@
         <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,10 +1958,10 @@
         <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,10 +1969,10 @@
         <v>46</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,10 +1980,10 @@
         <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,10 +1991,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1967,10 +2002,10 @@
         <v>51</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,10 +2013,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,10 +2024,10 @@
         <v>51</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,10 +2035,10 @@
         <v>55</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2011,10 +2046,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2022,10 +2057,10 @@
         <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,10 +2068,10 @@
         <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,10 +2079,10 @@
         <v>75</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,10 +2090,10 @@
         <v>79</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,10 +2101,10 @@
         <v>79</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,10 +2112,10 @@
         <v>79</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,10 +2123,10 @@
         <v>82</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2099,10 +2134,10 @@
         <v>82</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,10 +2145,10 @@
         <v>82</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,10 +2156,10 @@
         <v>85</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2132,10 +2167,10 @@
         <v>85</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,10 +2178,10 @@
         <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,10 +2189,10 @@
         <v>93</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,10 +2200,10 @@
         <v>101</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,10 +2211,10 @@
         <v>101</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,10 +2222,10 @@
         <v>101</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2198,10 +2233,10 @@
         <v>105</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2209,10 +2244,10 @@
         <v>105</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,10 +2255,10 @@
         <v>109</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,10 +2266,10 @@
         <v>114</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,10 +2277,10 @@
         <v>114</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,10 +2288,10 @@
         <v>114</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,10 +2299,10 @@
         <v>114</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,10 +2310,10 @@
         <v>114</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,10 +2321,10 @@
         <v>114</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,10 +2332,10 @@
         <v>114</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,10 +2343,10 @@
         <v>114</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,10 +2354,10 @@
         <v>117</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,10 +2365,10 @@
         <v>117</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,10 +2376,10 @@
         <v>120</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,10 +2387,10 @@
         <v>125</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,10 +2398,10 @@
         <v>130</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,10 +2409,10 @@
         <v>130</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,10 +2420,10 @@
         <v>134</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,10 +2431,10 @@
         <v>134</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,10 +2442,10 @@
         <v>134</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,10 +2453,10 @@
         <v>142</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,10 +2464,10 @@
         <v>145</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,10 +2475,10 @@
         <v>148</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,10 +2486,10 @@
         <v>150</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,10 +2497,10 @@
         <v>150</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,10 +2508,10 @@
         <v>153</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,10 +2519,10 @@
         <v>153</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,10 +2530,10 @@
         <v>153</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,10 +2541,32 @@
         <v>153</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>